<commit_message>
CEIP_1 Regulator Final Draft Drawing
</commit_message>
<xml_diff>
--- a/AE Zaid/Bagerhat/2021_22/Protecttive Work/Karamjol Protective Work/Design Data/Koromjol Cross Section.xlsx
+++ b/AE Zaid/Bagerhat/2021_22/Protecttive Work/Karamjol Protective Work/Design Data/Koromjol Cross Section.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,6 +111,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -158,7 +161,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -193,7 +196,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,13 +407,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="L326" sqref="L326"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -420,7 +423,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -428,7 +431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
         <v>0</v>
       </c>
@@ -436,7 +439,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C9" s="2">
         <v>5</v>
       </c>
@@ -444,7 +447,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
         <v>10</v>
       </c>
@@ -452,7 +455,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C11" s="2">
         <v>15</v>
       </c>
@@ -460,7 +463,7 @@
         <v>-2.0699999999999998</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C12" s="2">
         <v>20</v>
       </c>
@@ -468,7 +471,7 @@
         <v>-3.03</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C13" s="2">
         <v>25</v>
       </c>
@@ -476,7 +479,7 @@
         <v>-7.48</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C14" s="2">
         <v>30</v>
       </c>
@@ -484,7 +487,7 @@
         <v>-9.02</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C15" s="2">
         <v>35</v>
       </c>
@@ -492,7 +495,7 @@
         <v>-9.43</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C16" s="2">
         <v>40</v>
       </c>
@@ -500,7 +503,7 @@
         <v>-9.43</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="2">
         <v>45</v>
       </c>
@@ -508,7 +511,7 @@
         <v>-9.49</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="2">
         <v>50</v>
       </c>
@@ -516,7 +519,7 @@
         <v>-9.6199999999999992</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="2">
         <v>55</v>
       </c>
@@ -524,7 +527,7 @@
         <v>-9.52</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="2">
         <v>60</v>
       </c>
@@ -532,7 +535,7 @@
         <v>-9.4600000000000009</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="2">
         <v>65</v>
       </c>
@@ -540,7 +543,7 @@
         <v>-9.42</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" s="2">
         <v>70</v>
       </c>
@@ -548,7 +551,7 @@
         <v>-9.52</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="2">
         <v>75</v>
       </c>
@@ -556,7 +559,7 @@
         <v>-9.52</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" s="2">
         <v>80</v>
       </c>
@@ -564,7 +567,7 @@
         <v>-9.52</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" s="2">
         <v>85</v>
       </c>
@@ -572,7 +575,7 @@
         <v>-9.59</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="2">
         <v>90</v>
       </c>
@@ -580,7 +583,7 @@
         <v>-9.52</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" s="2">
         <v>95</v>
       </c>
@@ -588,7 +591,7 @@
         <v>-9.52</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" s="2">
         <v>100</v>
       </c>
@@ -596,7 +599,7 @@
         <v>-9.52</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" s="2">
         <v>105</v>
       </c>
@@ -604,7 +607,7 @@
         <v>-9.44</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30" s="2">
         <v>110</v>
       </c>
@@ -612,7 +615,7 @@
         <v>-9.41</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" s="2">
         <v>115</v>
       </c>
@@ -620,7 +623,7 @@
         <v>-9.41</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32" s="2">
         <v>120</v>
       </c>
@@ -628,7 +631,7 @@
         <v>-9.41</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="2">
         <v>125</v>
       </c>
@@ -636,7 +639,7 @@
         <v>-9.41</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" s="2">
         <v>130</v>
       </c>
@@ -644,7 +647,7 @@
         <v>-9.41</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" s="2">
         <v>135</v>
       </c>
@@ -652,7 +655,7 @@
         <v>-9.41</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" s="2">
         <v>140</v>
       </c>
@@ -660,7 +663,7 @@
         <v>-9.41</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C37" s="2">
         <v>145</v>
       </c>
@@ -668,7 +671,7 @@
         <v>-9.41</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38" s="2">
         <v>150</v>
       </c>
@@ -676,7 +679,7 @@
         <v>-9.49</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39" s="2">
         <v>155</v>
       </c>
@@ -684,7 +687,7 @@
         <v>-9.51</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" s="2">
         <v>160</v>
       </c>
@@ -692,7 +695,7 @@
         <v>-9.59</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" s="2">
         <v>165</v>
       </c>
@@ -700,7 +703,7 @@
         <v>-9.51</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" s="2">
         <v>170</v>
       </c>
@@ -708,7 +711,7 @@
         <v>-9.51</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" s="2">
         <v>175</v>
       </c>
@@ -716,7 +719,7 @@
         <v>-9.5</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44" s="2">
         <v>180</v>
       </c>
@@ -724,7 +727,7 @@
         <v>-9.59</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45" s="2">
         <v>185</v>
       </c>
@@ -732,7 +735,7 @@
         <v>-9.52</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46" s="2">
         <v>190</v>
       </c>
@@ -740,7 +743,7 @@
         <v>-9.6</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C47" s="2">
         <v>195</v>
       </c>
@@ -748,7 +751,7 @@
         <v>-9.6</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C48" s="2">
         <v>200</v>
       </c>
@@ -756,7 +759,7 @@
         <v>-9.59</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
         <v>3</v>
       </c>
@@ -767,7 +770,7 @@
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
         <v>1</v>
       </c>
@@ -775,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C56" s="2">
         <v>0</v>
       </c>
@@ -783,7 +786,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C57" s="2">
         <v>5</v>
       </c>
@@ -791,7 +794,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C58" s="2">
         <v>10</v>
       </c>
@@ -799,7 +802,7 @@
         <v>-0.43</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C59" s="2">
         <v>15</v>
       </c>
@@ -807,7 +810,7 @@
         <v>-1.53</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C60" s="2">
         <v>20</v>
       </c>
@@ -815,7 +818,7 @@
         <v>-2.76</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C61" s="2">
         <v>25</v>
       </c>
@@ -823,7 +826,7 @@
         <v>-5.74</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C62" s="2">
         <v>30</v>
       </c>
@@ -831,7 +834,7 @@
         <v>-9.77</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C63" s="2">
         <v>35</v>
       </c>
@@ -839,7 +842,7 @@
         <v>-9.77</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C64" s="2">
         <v>40</v>
       </c>
@@ -847,7 +850,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65" s="2">
         <v>45</v>
       </c>
@@ -855,7 +858,7 @@
         <v>-10.199999999999999</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" s="2">
         <v>50</v>
       </c>
@@ -863,7 +866,7 @@
         <v>-10.220000000000001</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" s="2">
         <v>55</v>
       </c>
@@ -871,7 +874,7 @@
         <v>-10.199999999999999</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" s="2">
         <v>60</v>
       </c>
@@ -879,7 +882,7 @@
         <v>-10.28</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" s="2">
         <v>65</v>
       </c>
@@ -887,7 +890,7 @@
         <v>-10.029999999999999</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" s="2">
         <v>70</v>
       </c>
@@ -895,7 +898,7 @@
         <v>-10.08</v>
       </c>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C71" s="2">
         <v>75</v>
       </c>
@@ -903,7 +906,7 @@
         <v>-10.029999999999999</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C72" s="2">
         <v>80</v>
       </c>
@@ -911,7 +914,7 @@
         <v>-9.83</v>
       </c>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C73" s="2">
         <v>85</v>
       </c>
@@ -919,7 +922,7 @@
         <v>-9.83</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C74" s="2">
         <v>90</v>
       </c>
@@ -927,7 +930,7 @@
         <v>-9.82</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C75" s="2">
         <v>95</v>
       </c>
@@ -935,7 +938,7 @@
         <v>-9.73</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C76" s="2">
         <v>100</v>
       </c>
@@ -943,7 +946,7 @@
         <v>-9.68</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C77" s="2">
         <v>105</v>
       </c>
@@ -951,7 +954,7 @@
         <v>-9.7100000000000009</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C78" s="2">
         <v>110</v>
       </c>
@@ -959,7 +962,7 @@
         <v>-9.5500000000000007</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C79" s="2">
         <v>115</v>
       </c>
@@ -967,7 +970,7 @@
         <v>-9.56</v>
       </c>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C80" s="2">
         <v>120</v>
       </c>
@@ -975,7 +978,7 @@
         <v>-9.5299999999999994</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C81" s="2">
         <v>125</v>
       </c>
@@ -983,7 +986,7 @@
         <v>-9.6199999999999992</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C82" s="2">
         <v>130</v>
       </c>
@@ -991,7 +994,7 @@
         <v>-9.64</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" s="2">
         <v>135</v>
       </c>
@@ -999,7 +1002,7 @@
         <v>-9.69</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" s="2">
         <v>140</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>-9.74</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C85" s="2">
         <v>145</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>-9.74</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C86" s="2">
         <v>150</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>-9.83</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C87" s="2">
         <v>155</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>-9.74</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C88" s="2">
         <v>160</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>-9.77</v>
       </c>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C89" s="2">
         <v>165</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>-9.85</v>
       </c>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C90" s="2">
         <v>170</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>-9.85</v>
       </c>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C91" s="2">
         <v>175</v>
       </c>
@@ -1063,7 +1066,7 @@
         <v>-9.85</v>
       </c>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C92" s="2">
         <v>180</v>
       </c>
@@ -1071,7 +1074,7 @@
         <v>-9.8000000000000007</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C93" s="2">
         <v>185</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>-9.86</v>
       </c>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C94" s="2">
         <v>190</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>-9.76</v>
       </c>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C95" s="2">
         <v>195</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>-9.77</v>
       </c>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C96" s="2">
         <v>200</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>-9.65</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C97" s="2">
         <v>205</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>-9.94</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C98" s="2">
         <v>210</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>-9.76</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C99" s="2">
         <v>215</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>-9.66</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C100" s="2">
         <v>220</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>-9.6</v>
       </c>
     </row>
-    <row r="104" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B104" s="4" t="s">
         <v>4</v>
       </c>
@@ -1146,7 +1149,7 @@
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C106" t="s">
         <v>1</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C108" s="2">
         <v>0</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C109" s="2">
         <v>5</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C110" s="2">
         <v>10</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>-0.91</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C111" s="2">
         <v>15</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C112" s="2">
         <v>20</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>-6.37</v>
       </c>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C113" s="2">
         <v>25</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>-9.77</v>
       </c>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C114" s="2">
         <v>30</v>
       </c>
@@ -1210,7 +1213,7 @@
         <v>-10.58</v>
       </c>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C115" s="2">
         <v>35</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>-10.39</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C116" s="2">
         <v>40</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>-10.47</v>
       </c>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C117" s="2">
         <v>45</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>-10.54</v>
       </c>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C118" s="2">
         <v>50</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>-10.44</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C119" s="2">
         <v>55</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>-10.44</v>
       </c>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C120" s="2">
         <v>60</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>-10.42</v>
       </c>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C121" s="2">
         <v>65</v>
       </c>
@@ -1266,7 +1269,7 @@
         <v>-10.24</v>
       </c>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C122" s="2">
         <v>70</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>-10.09</v>
       </c>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C123" s="2">
         <v>75</v>
       </c>
@@ -1282,7 +1285,7 @@
         <v>-10.17</v>
       </c>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C124" s="2">
         <v>80</v>
       </c>
@@ -1290,7 +1293,7 @@
         <v>-10.039999999999999</v>
       </c>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C125" s="2">
         <v>85</v>
       </c>
@@ -1298,7 +1301,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C126" s="2">
         <v>90</v>
       </c>
@@ -1306,7 +1309,7 @@
         <v>-9.7899999999999991</v>
       </c>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C127" s="2">
         <v>95</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>-9.6999999999999993</v>
       </c>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C128" s="2">
         <v>100</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C129" s="2">
         <v>105</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>-9.89</v>
       </c>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C130" s="2">
         <v>110</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C131" s="2">
         <v>115</v>
       </c>
@@ -1346,7 +1349,7 @@
         <v>-9.67</v>
       </c>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C132" s="2">
         <v>120</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>-9.8000000000000007</v>
       </c>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C133" s="2">
         <v>125</v>
       </c>
@@ -1362,7 +1365,7 @@
         <v>-9.89</v>
       </c>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C134" s="2">
         <v>130</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>-9.98</v>
       </c>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C135" s="2">
         <v>135</v>
       </c>
@@ -1378,7 +1381,7 @@
         <v>-9.98</v>
       </c>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C136" s="2">
         <v>140</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>-9.98</v>
       </c>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C137" s="2">
         <v>145</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>-9.98</v>
       </c>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C138" s="2">
         <v>150</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>-9.92</v>
       </c>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C139" s="2">
         <v>155</v>
       </c>
@@ -1410,7 +1413,7 @@
         <v>-9.8800000000000008</v>
       </c>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C140" s="2">
         <v>160</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>-9.8000000000000007</v>
       </c>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C141" s="2">
         <v>165</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>-9.89</v>
       </c>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C142" s="2">
         <v>170</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>-9.6999999999999993</v>
       </c>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C143" s="2">
         <v>175</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C144" s="2">
         <v>180</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C145" s="2">
         <v>185</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>-9.77</v>
       </c>
     </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C146" s="2">
         <v>190</v>
       </c>
@@ -1466,19 +1469,19 @@
         <v>-9.6199999999999992</v>
       </c>
     </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C147" s="2"/>
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C148" s="2"/>
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C149" s="2"/>
       <c r="D149" s="3"/>
     </row>
-    <row r="150" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B150" s="4" t="s">
         <v>5</v>
       </c>
@@ -1489,11 +1492,11 @@
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
     </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C151" s="2"/>
       <c r="D151" s="3"/>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C152" t="s">
         <v>1</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C154" s="2">
         <v>0</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C155" s="2">
         <v>5</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C156" s="2">
         <v>10</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C157" s="2">
         <v>15</v>
       </c>
@@ -1533,7 +1536,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C158" s="2">
         <v>20</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>-3.54</v>
       </c>
     </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C159" s="2">
         <v>25</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>-6.34</v>
       </c>
     </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C160" s="2">
         <v>30</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>-7.29</v>
       </c>
     </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C161" s="2">
         <v>35</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>-9.19</v>
       </c>
     </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C162" s="2">
         <v>40</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>-9.85</v>
       </c>
     </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C163" s="2">
         <v>45</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>-10.27</v>
       </c>
     </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C164" s="2">
         <v>50</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>-10.53</v>
       </c>
     </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C165" s="2">
         <v>55</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>-10.79</v>
       </c>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C166" s="2">
         <v>60</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>-10.81</v>
       </c>
     </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C167" s="2">
         <v>65</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>-10.62</v>
       </c>
     </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C168" s="2">
         <v>70</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>-11.01</v>
       </c>
     </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C169" s="2">
         <v>75</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>-11.03</v>
       </c>
     </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C170" s="2">
         <v>80</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>-11.2</v>
       </c>
     </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C171" s="2">
         <v>85</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>-10.88</v>
       </c>
     </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C172" s="2">
         <v>90</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>-10.81</v>
       </c>
     </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C173" s="2">
         <v>95</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>-10.62</v>
       </c>
     </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C174" s="2">
         <v>100</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>-10.57</v>
       </c>
     </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C175" s="2">
         <v>105</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>-10.46</v>
       </c>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C176" s="2">
         <v>110</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>-10.41</v>
       </c>
     </row>
-    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C177" s="2">
         <v>115</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>-10.42</v>
       </c>
     </row>
-    <row r="178" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C178" s="2">
         <v>120</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>-10.32</v>
       </c>
     </row>
-    <row r="179" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C179" s="2">
         <v>125</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>-10.3</v>
       </c>
     </row>
-    <row r="180" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C180" s="2">
         <v>130</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>-10.14</v>
       </c>
     </row>
-    <row r="181" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C181" s="2">
         <v>135</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>-10.06</v>
       </c>
     </row>
-    <row r="182" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C182" s="2">
         <v>140</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>-10.029999999999999</v>
       </c>
     </row>
-    <row r="183" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C183" s="2">
         <v>145</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>-9.92</v>
       </c>
     </row>
-    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C184" s="2">
         <v>150</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>-9.92</v>
       </c>
     </row>
-    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C185" s="2">
         <v>155</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C186" s="2">
         <v>160</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>-9.92</v>
       </c>
     </row>
-    <row r="187" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C187" s="2">
         <v>165</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>-9.9499999999999993</v>
       </c>
     </row>
-    <row r="188" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C188" s="2">
         <v>170</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>-9.99</v>
       </c>
     </row>
-    <row r="189" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C189" s="2">
         <v>175</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>-9.82</v>
       </c>
     </row>
-    <row r="190" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C190" s="2">
         <v>180</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>-9.8699999999999992</v>
       </c>
     </row>
-    <row r="191" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C191" s="2">
         <v>185</v>
       </c>
@@ -1805,7 +1808,7 @@
         <v>-9.92</v>
       </c>
     </row>
-    <row r="192" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C192" s="2">
         <v>190</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>-9.92</v>
       </c>
     </row>
-    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C193" s="2">
         <v>195</v>
       </c>
@@ -1821,7 +1824,7 @@
         <v>-9.83</v>
       </c>
     </row>
-    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C194" s="2">
         <v>200</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>-9.92</v>
       </c>
     </row>
-    <row r="198" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B198" s="4" t="s">
         <v>6</v>
       </c>
@@ -1840,7 +1843,7 @@
       <c r="G198" s="4"/>
       <c r="H198" s="4"/>
     </row>
-    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C200" t="s">
         <v>1</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C202" s="2">
         <v>0</v>
       </c>
@@ -1856,7 +1859,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="203" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C203" s="2">
         <v>5</v>
       </c>
@@ -1864,7 +1867,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="204" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C204" s="2">
         <v>10</v>
       </c>
@@ -1872,7 +1875,7 @@
         <v>-1.58</v>
       </c>
     </row>
-    <row r="205" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C205" s="2">
         <v>15</v>
       </c>
@@ -1880,7 +1883,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="206" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C206" s="2">
         <v>20</v>
       </c>
@@ -1888,7 +1891,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="207" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C207" s="2">
         <v>25</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>-7.63</v>
       </c>
     </row>
-    <row r="208" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C208" s="2">
         <v>30</v>
       </c>
@@ -1904,7 +1907,7 @@
         <v>-10.7</v>
       </c>
     </row>
-    <row r="209" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C209" s="2">
         <v>35</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>-11.09</v>
       </c>
     </row>
-    <row r="210" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C210" s="2">
         <v>40</v>
       </c>
@@ -1920,7 +1923,7 @@
         <v>-11.29</v>
       </c>
     </row>
-    <row r="211" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C211" s="2">
         <v>45</v>
       </c>
@@ -1928,7 +1931,7 @@
         <v>-11.45</v>
       </c>
     </row>
-    <row r="212" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C212" s="2">
         <v>50</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>-11.32</v>
       </c>
     </row>
-    <row r="213" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C213" s="2">
         <v>55</v>
       </c>
@@ -1944,7 +1947,7 @@
         <v>-11.39</v>
       </c>
     </row>
-    <row r="214" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C214" s="2">
         <v>60</v>
       </c>
@@ -1952,7 +1955,7 @@
         <v>-11.29</v>
       </c>
     </row>
-    <row r="215" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C215" s="2">
         <v>65</v>
       </c>
@@ -1960,7 +1963,7 @@
         <v>-11.29</v>
       </c>
     </row>
-    <row r="216" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C216" s="2">
         <v>70</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>-11.5</v>
       </c>
     </row>
-    <row r="217" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C217" s="2">
         <v>75</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>-11.48</v>
       </c>
     </row>
-    <row r="218" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C218" s="2">
         <v>80</v>
       </c>
@@ -1984,7 +1987,7 @@
         <v>-11.25</v>
       </c>
     </row>
-    <row r="219" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C219" s="2">
         <v>85</v>
       </c>
@@ -1992,7 +1995,7 @@
         <v>-10.91</v>
       </c>
     </row>
-    <row r="220" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C220" s="2">
         <v>90</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>-10.7</v>
       </c>
     </row>
-    <row r="221" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C221" s="2">
         <v>95</v>
       </c>
@@ -2008,7 +2011,7 @@
         <v>-10.56</v>
       </c>
     </row>
-    <row r="222" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C222" s="2">
         <v>100</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>-10.46</v>
       </c>
     </row>
-    <row r="223" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C223" s="2">
         <v>105</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>-10.32</v>
       </c>
     </row>
-    <row r="224" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C224" s="2">
         <v>110</v>
       </c>
@@ -2032,7 +2035,7 @@
         <v>-10.28</v>
       </c>
     </row>
-    <row r="225" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C225" s="2">
         <v>115</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>-10.210000000000001</v>
       </c>
     </row>
-    <row r="226" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C226" s="2">
         <v>120</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>-10.18</v>
       </c>
     </row>
-    <row r="227" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C227" s="2">
         <v>125</v>
       </c>
@@ -2056,7 +2059,7 @@
         <v>-10.07</v>
       </c>
     </row>
-    <row r="228" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C228" s="2">
         <v>130</v>
       </c>
@@ -2064,7 +2067,7 @@
         <v>-9.98</v>
       </c>
     </row>
-    <row r="229" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C229" s="2">
         <v>135</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>-9.81</v>
       </c>
     </row>
-    <row r="230" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C230" s="2">
         <v>140</v>
       </c>
@@ -2080,7 +2083,7 @@
         <v>-9.8699999999999992</v>
       </c>
     </row>
-    <row r="231" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C231" s="2">
         <v>145</v>
       </c>
@@ -2088,7 +2091,7 @@
         <v>-9.8699999999999992</v>
       </c>
     </row>
-    <row r="232" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C232" s="2">
         <v>150</v>
       </c>
@@ -2096,7 +2099,7 @@
         <v>-9.9700000000000006</v>
       </c>
     </row>
-    <row r="233" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C233" s="2">
         <v>155</v>
       </c>
@@ -2104,7 +2107,7 @@
         <v>-10.18</v>
       </c>
     </row>
-    <row r="234" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C234" s="2">
         <v>160</v>
       </c>
@@ -2112,7 +2115,7 @@
         <v>-10.18</v>
       </c>
     </row>
-    <row r="235" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C235" s="2">
         <v>165</v>
       </c>
@@ -2120,7 +2123,7 @@
         <v>-10.18</v>
       </c>
     </row>
-    <row r="236" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C236" s="2">
         <v>170</v>
       </c>
@@ -2128,7 +2131,7 @@
         <v>-10.18</v>
       </c>
     </row>
-    <row r="237" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C237" s="2">
         <v>175</v>
       </c>
@@ -2136,7 +2139,7 @@
         <v>-10.37</v>
       </c>
     </row>
-    <row r="238" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C238" s="2">
         <v>180</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>-10.18</v>
       </c>
     </row>
-    <row r="239" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C239" s="2">
         <v>185</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>-10.08</v>
       </c>
     </row>
-    <row r="240" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C240" s="2">
         <v>190</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>-10.19</v>
       </c>
     </row>
-    <row r="241" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C241" s="2">
         <v>195</v>
       </c>
@@ -2168,11 +2171,11 @@
         <v>-10.39</v>
       </c>
     </row>
-    <row r="242" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C242" s="2"/>
       <c r="D242" s="3"/>
     </row>
-    <row r="245" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B245" s="4" t="s">
         <v>7</v>
       </c>
@@ -2183,7 +2186,7 @@
       <c r="G245" s="4"/>
       <c r="H245" s="4"/>
     </row>
-    <row r="247" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C247" t="s">
         <v>1</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C249" s="2">
         <v>0</v>
       </c>
@@ -2199,7 +2202,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="250" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C250" s="2">
         <v>5</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="251" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C251" s="2">
         <v>10</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="252" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C252" s="2">
         <v>15</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="253" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C253" s="2">
         <v>20</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="254" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C254" s="2">
         <v>25</v>
       </c>
@@ -2239,7 +2242,7 @@
         <v>-0.37</v>
       </c>
     </row>
-    <row r="255" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C255" s="2">
         <v>30</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>-2.1800000000000002</v>
       </c>
     </row>
-    <row r="256" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C256" s="2">
         <v>35</v>
       </c>
@@ -2255,7 +2258,7 @@
         <v>-5.34</v>
       </c>
     </row>
-    <row r="257" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C257" s="2">
         <v>40</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>-7.56</v>
       </c>
     </row>
-    <row r="258" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C258" s="2">
         <v>45</v>
       </c>
@@ -2271,7 +2274,7 @@
         <v>-9.0299999999999994</v>
       </c>
     </row>
-    <row r="259" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C259" s="2">
         <v>50</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>-9.49</v>
       </c>
     </row>
-    <row r="260" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C260" s="2">
         <v>55</v>
       </c>
@@ -2287,7 +2290,7 @@
         <v>-9.69</v>
       </c>
     </row>
-    <row r="261" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C261" s="2">
         <v>60</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>-10.65</v>
       </c>
     </row>
-    <row r="262" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C262" s="2">
         <v>65</v>
       </c>
@@ -2303,7 +2306,7 @@
         <v>-12.5</v>
       </c>
     </row>
-    <row r="263" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C263" s="2">
         <v>70</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>-13.57</v>
       </c>
     </row>
-    <row r="264" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C264" s="2">
         <v>75</v>
       </c>
@@ -2319,7 +2322,7 @@
         <v>-13.94</v>
       </c>
     </row>
-    <row r="265" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C265" s="2">
         <v>80</v>
       </c>
@@ -2327,7 +2330,7 @@
         <v>-13.27</v>
       </c>
     </row>
-    <row r="266" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C266" s="2">
         <v>85</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>-12.43</v>
       </c>
     </row>
-    <row r="267" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C267" s="2">
         <v>90</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>-11.81</v>
       </c>
     </row>
-    <row r="268" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C268" s="2">
         <v>95</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>-11.14</v>
       </c>
     </row>
-    <row r="269" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C269" s="2">
         <v>100</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>-10.54</v>
       </c>
     </row>
-    <row r="270" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C270" s="2">
         <v>105</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>-10.199999999999999</v>
       </c>
     </row>
-    <row r="271" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C271" s="2">
         <v>110</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>-9.98</v>
       </c>
     </row>
-    <row r="272" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C272" s="2">
         <v>115</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>-9.85</v>
       </c>
     </row>
-    <row r="273" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C273" s="2">
         <v>120</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>-9.76</v>
       </c>
     </row>
-    <row r="274" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C274" s="2">
         <v>125</v>
       </c>
@@ -2399,7 +2402,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="275" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C275" s="2">
         <v>130</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>-9.86</v>
       </c>
     </row>
-    <row r="276" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C276" s="2">
         <v>135</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>-9.86</v>
       </c>
     </row>
-    <row r="277" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C277" s="2">
         <v>140</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>-9.86</v>
       </c>
     </row>
-    <row r="278" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C278" s="2">
         <v>145</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>-9.76</v>
       </c>
     </row>
-    <row r="279" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C279" s="2">
         <v>150</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>-9.9700000000000006</v>
       </c>
     </row>
-    <row r="280" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C280" s="2">
         <v>155</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>-10.06</v>
       </c>
     </row>
-    <row r="281" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C281" s="2">
         <v>160</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>-10.06</v>
       </c>
     </row>
-    <row r="282" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C282" s="2">
         <v>165</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>-9.98</v>
       </c>
     </row>
-    <row r="283" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C283" s="2">
         <v>170</v>
       </c>
@@ -2471,7 +2474,7 @@
         <v>-10.050000000000001</v>
       </c>
     </row>
-    <row r="284" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C284" s="2">
         <v>175</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>-10.050000000000001</v>
       </c>
     </row>
-    <row r="285" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C285" s="2">
         <v>180</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>-10.26</v>
       </c>
     </row>
-    <row r="286" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C286" s="2">
         <v>185</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>-10.26</v>
       </c>
     </row>
-    <row r="287" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C287" s="2">
         <v>190</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>-10.26</v>
       </c>
     </row>
-    <row r="288" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C288" s="2">
         <v>195</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>-10.26</v>
       </c>
     </row>
-    <row r="289" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C289" s="2">
         <v>200</v>
       </c>
@@ -2519,7 +2522,7 @@
         <v>-10.26</v>
       </c>
     </row>
-    <row r="290" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C290" s="2">
         <v>205</v>
       </c>
@@ -2527,7 +2530,7 @@
         <v>-10.26</v>
       </c>
     </row>
-    <row r="291" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C291" s="2">
         <v>210</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>-10.16</v>
       </c>
     </row>
-    <row r="292" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C292" s="2">
         <v>215</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>-10.199999999999999</v>
       </c>
     </row>
-    <row r="293" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C293" s="2">
         <v>220</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>-10.25</v>
       </c>
     </row>
-    <row r="297" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B297" s="4" t="s">
         <v>8</v>
       </c>
@@ -2562,7 +2565,7 @@
       <c r="G297" s="4"/>
       <c r="H297" s="4"/>
     </row>
-    <row r="299" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C299" t="s">
         <v>1</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C301" s="2">
         <v>0</v>
       </c>
@@ -2578,7 +2581,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="302" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C302" s="2">
         <v>5</v>
       </c>
@@ -2586,7 +2589,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="303" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C303" s="2">
         <v>10</v>
       </c>
@@ -2594,7 +2597,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="304" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C304" s="2">
         <v>15</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>-0.03</v>
       </c>
     </row>
-    <row r="305" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C305" s="2">
         <v>20</v>
       </c>
@@ -2610,7 +2613,7 @@
         <v>-1.66</v>
       </c>
     </row>
-    <row r="306" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C306" s="2">
         <v>25</v>
       </c>
@@ -2618,7 +2621,7 @@
         <v>-2.5299999999999998</v>
       </c>
     </row>
-    <row r="307" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C307" s="2">
         <v>30</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>-3.85</v>
       </c>
     </row>
-    <row r="308" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C308" s="2">
         <v>35</v>
       </c>
@@ -2634,7 +2637,7 @@
         <v>-3.98</v>
       </c>
     </row>
-    <row r="309" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C309" s="2">
         <v>40</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>-3.75</v>
       </c>
     </row>
-    <row r="310" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C310" s="2">
         <v>45</v>
       </c>
@@ -2650,7 +2653,7 @@
         <v>-3.04</v>
       </c>
     </row>
-    <row r="311" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C311" s="2">
         <v>50</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>-1.47</v>
       </c>
     </row>
-    <row r="312" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C312" s="2">
         <v>55</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="313" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C313" s="2">
         <v>60</v>
       </c>
@@ -2674,7 +2677,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="314" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C314" s="2">
         <v>65</v>
       </c>
@@ -2682,7 +2685,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="315" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C315" s="2">
         <v>70</v>
       </c>
@@ -2690,7 +2693,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="318" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B318" s="4" t="s">
         <v>9</v>
       </c>
@@ -2701,7 +2704,7 @@
       <c r="G318" s="4"/>
       <c r="H318" s="4"/>
     </row>
-    <row r="320" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C320" t="s">
         <v>1</v>
       </c>
@@ -2709,7 +2712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C322" s="2">
         <v>0</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="323" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C323" s="2">
         <v>5</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="324" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C324" s="2">
         <v>10</v>
       </c>
@@ -2733,7 +2736,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="325" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C325" s="2">
         <v>15</v>
       </c>
@@ -2741,7 +2744,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="326" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C326" s="2">
         <v>20</v>
       </c>
@@ -2749,7 +2752,7 @@
         <v>-1.38</v>
       </c>
     </row>
-    <row r="327" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C327" s="2">
         <v>25</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>-1.89</v>
       </c>
     </row>
-    <row r="328" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C328" s="2">
         <v>30</v>
       </c>
@@ -2765,7 +2768,7 @@
         <v>-3.69</v>
       </c>
     </row>
-    <row r="329" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C329" s="2">
         <v>35</v>
       </c>
@@ -2773,7 +2776,7 @@
         <v>-3.58</v>
       </c>
     </row>
-    <row r="330" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C330" s="2">
         <v>40</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>-3.19</v>
       </c>
     </row>
-    <row r="331" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C331" s="2">
         <v>45</v>
       </c>
@@ -2789,7 +2792,7 @@
         <v>-1.81</v>
       </c>
     </row>
-    <row r="332" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C332" s="2">
         <v>50</v>
       </c>
@@ -2797,7 +2800,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="333" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C333" s="2">
         <v>55</v>
       </c>
@@ -2805,7 +2808,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="334" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C334" s="2">
         <v>60</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="335" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C335" s="2">
         <v>65</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="336" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C336" s="2">
         <v>70</v>
       </c>
@@ -2849,9 +2852,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2863,7 +2868,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>